<commit_message>
2 bug has been added into bug file
</commit_message>
<xml_diff>
--- a/Gigalogy_Task.xlsx
+++ b/Gigalogy_Task.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6800"/>
+    <workbookView windowWidth="19200" windowHeight="6080" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Part_A_API_Testing" sheetId="1" r:id="rId1"/>
+    <sheet name="Part_C_Bug_Report" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="69">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -269,6 +270,21 @@
   </si>
   <si>
     <t>Shirt item has been displayed according to max price review_count first</t>
+  </si>
+  <si>
+    <t>Bug ID</t>
+  </si>
+  <si>
+    <t>Bug Title</t>
+  </si>
+  <si>
+    <t>Steps to reproduce</t>
+  </si>
+  <si>
+    <t>Severity</t>
+  </si>
+  <si>
+    <t>Priority</t>
   </si>
 </sst>
 </file>
@@ -457,6 +473,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -464,12 +486,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -916,29 +932,26 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1479,308 +1492,412 @@
   <sheetPr/>
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="12.0909090909091" style="3" customWidth="1"/>
-    <col min="2" max="2" width="31.9090909090909" style="3" customWidth="1"/>
-    <col min="3" max="3" width="18.3636363636364" style="3" customWidth="1"/>
-    <col min="4" max="4" width="28.6363636363636" style="3" customWidth="1"/>
-    <col min="5" max="5" width="26.3636363636364" style="3" customWidth="1"/>
-    <col min="6" max="6" width="28" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="8.72727272727273" style="3"/>
+    <col min="1" max="1" width="12.0909090909091" style="2" customWidth="1"/>
+    <col min="2" max="2" width="31.9090909090909" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.3636363636364" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.6363636363636" style="2" customWidth="1"/>
+    <col min="5" max="5" width="26.3636363636364" style="2" customWidth="1"/>
+    <col min="6" max="6" width="28" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.72727272727273" style="2"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:8">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" s="2" customFormat="1" ht="174" spans="1:8">
-      <c r="A2" s="3" t="s">
+    <row r="2" s="5" customFormat="1" ht="174" spans="1:7">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="7"/>
     </row>
     <row r="3" ht="58" spans="1:7">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" ht="58" spans="1:7">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" ht="58" spans="1:7">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" ht="101.5" spans="1:7">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="7" ht="116" spans="1:7">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="8" ht="116" spans="1:7">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" ht="130.5" spans="1:7">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="10" ht="130.5" spans="1:7">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" ht="130.5" spans="1:7">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="12" ht="130.5" spans="1:7">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="7:7">
-      <c r="G13" s="7"/>
+      <c r="G13" s="5"/>
     </row>
     <row r="14" spans="7:7">
-      <c r="G14" s="7"/>
+      <c r="G14" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="2"/>
+  <cols>
+    <col min="2" max="2" width="12.2727272727273" customWidth="1"/>
+    <col min="3" max="3" width="17.8181818181818" customWidth="1"/>
+    <col min="4" max="4" width="16.8181818181818" customWidth="1"/>
+    <col min="5" max="5" width="17.8181818181818" customWidth="1"/>
+    <col min="6" max="6" width="15.1818181818182" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" ht="101.5" spans="1:10">
+      <c r="A2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" ht="116" spans="1:9">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
test case added for UI testing
</commit_message>
<xml_diff>
--- a/Gigalogy_Task.xlsx
+++ b/Gigalogy_Task.xlsx
@@ -4,11 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6080" activeTab="1"/>
+    <workbookView windowWidth="18350" windowHeight="6800" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Part_A_API_Testing" sheetId="1" r:id="rId1"/>
     <sheet name="Part_C_Bug_Report" sheetId="2" r:id="rId2"/>
+    <sheet name="Part_D_basic_performance_check" sheetId="3" r:id="rId3"/>
+    <sheet name="Part_B_Web_UI" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="110">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -285,6 +287,129 @@
   </si>
   <si>
     <t>Priority</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>From API testing</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Significance</t>
+  </si>
+  <si>
+    <t>Thread users</t>
+  </si>
+  <si>
+    <t>50 virtual users</t>
+  </si>
+  <si>
+    <t>ramp up</t>
+  </si>
+  <si>
+    <t>5 sec</t>
+  </si>
+  <si>
+    <t>50/5 = 10 users per sec will be executed</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>average response time of 21.5 seconds</t>
+  </si>
+  <si>
+    <t>90% of requests completed within 34.8 seconds</t>
+  </si>
+  <si>
+    <t>95% of requests completed within 35.7 seconds</t>
+  </si>
+  <si>
+    <t>99% of requests completed within 37.2 seconds</t>
+  </si>
+  <si>
+    <t>Error %</t>
+  </si>
+  <si>
+    <t>No api request has been failed, each one has been succeeded</t>
+  </si>
+  <si>
+    <t>Throughput</t>
+  </si>
+  <si>
+    <t>about 1.2 requests were processed each second</t>
+  </si>
+  <si>
+    <t>Search a product by product name</t>
+  </si>
+  <si>
+    <t>tops</t>
+  </si>
+  <si>
+    <t>1. Go to the website. 2. Enter search item into the search box. 3. Hit enter or click Search button</t>
+  </si>
+  <si>
+    <t>Relevant products should be displayed</t>
+  </si>
+  <si>
+    <t>Same as expected, all tops has been displayed</t>
+  </si>
+  <si>
+    <t>Search a product by product image</t>
+  </si>
+  <si>
+    <t>1. Go to the website. 2. Click camera icon right side of the search box 3. Upload image of the product.</t>
+  </si>
+  <si>
+    <t>Relevant product should be displayed</t>
+  </si>
+  <si>
+    <t>Browse Product detail page</t>
+  </si>
+  <si>
+    <t>1. Go to the website. 2. Navigate to a product.</t>
+  </si>
+  <si>
+    <t>Product details should be displayed in a popup window</t>
+  </si>
+  <si>
+    <t>Same as expected, product image, Title, description, add to cart has been displayed along with other product details</t>
+  </si>
+  <si>
+    <t>Test "add to shopping cart" button in product display page</t>
+  </si>
+  <si>
+    <t>1. Go to the website. 2.  Navigate to product detail page. 3. Click "add to shopping cart" button.</t>
+  </si>
+  <si>
+    <t>1 should be displayed with increment and decrement option instead of "add to shopping cart"</t>
+  </si>
+  <si>
+    <t>Test shopping cart page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Go to the website. 2.  Navigate to product detail page. 3. Click "add to shopping cart" button. 4. Navigate to shopping cart page. </t>
+  </si>
+  <si>
+    <t>Added product should be displayed here.</t>
+  </si>
+  <si>
+    <t>Click "Load More" multiple time.</t>
+  </si>
+  <si>
+    <t>1. Go to the website. 2. Navigate to the bottom portion of the page. 3. Click load more multiple time.</t>
+  </si>
+  <si>
+    <t>More products should be displayed on each click.</t>
   </si>
 </sst>
 </file>
@@ -473,6 +598,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -480,12 +611,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -932,7 +1057,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -942,19 +1067,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1232,6 +1369,53 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>205105</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>151765</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>540385</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>5715</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="205105" y="1809115"/>
+          <a:ext cx="7498080" cy="2432050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
@@ -1495,18 +1679,18 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="$A1:$XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="12.0909090909091" style="2" customWidth="1"/>
-    <col min="2" max="2" width="31.9090909090909" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.3636363636364" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.6363636363636" style="2" customWidth="1"/>
-    <col min="5" max="5" width="26.3636363636364" style="2" customWidth="1"/>
-    <col min="6" max="6" width="28" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.72727272727273" style="2"/>
+    <col min="1" max="1" width="12.0909090909091" style="7" customWidth="1"/>
+    <col min="2" max="2" width="31.9090909090909" style="7" customWidth="1"/>
+    <col min="3" max="3" width="18.3636363636364" style="7" customWidth="1"/>
+    <col min="4" max="4" width="28.6363636363636" style="7" customWidth="1"/>
+    <col min="5" max="5" width="26.3636363636364" style="7" customWidth="1"/>
+    <col min="6" max="6" width="28" style="7" customWidth="1"/>
+    <col min="7" max="16384" width="8.72727272727273" style="7"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:8">
@@ -1535,264 +1719,264 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" s="5" customFormat="1" ht="174" spans="1:7">
-      <c r="A2" s="2" t="s">
+    <row r="2" s="9" customFormat="1" ht="174" spans="1:7">
+      <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" ht="58" spans="1:7">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" ht="58" spans="1:7">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" ht="58" spans="1:7">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" ht="101.5" spans="1:7">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="8" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="7" ht="116" spans="1:7">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="8" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="8" ht="116" spans="1:7">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" ht="130.5" spans="1:7">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="8" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="10" ht="130.5" spans="1:7">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" ht="130.5" spans="1:7">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="8" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="12" ht="130.5" spans="1:7">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="7:7">
-      <c r="G13" s="5"/>
+      <c r="G13" s="9"/>
     </row>
     <row r="14" spans="7:7">
-      <c r="G14" s="5"/>
+      <c r="G14" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1805,17 +1989,21 @@
   <sheetPr/>
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="2"/>
   <cols>
-    <col min="2" max="2" width="12.2727272727273" customWidth="1"/>
-    <col min="3" max="3" width="17.8181818181818" customWidth="1"/>
-    <col min="4" max="4" width="16.8181818181818" customWidth="1"/>
-    <col min="5" max="5" width="17.8181818181818" customWidth="1"/>
-    <col min="6" max="6" width="15.1818181818182" customWidth="1"/>
+    <col min="1" max="1" width="8.72727272727273" style="2"/>
+    <col min="2" max="2" width="12.2727272727273" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.8181818181818" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.8181818181818" style="2" customWidth="1"/>
+    <col min="5" max="5" width="17.8181818181818" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.1818181818182" style="2" customWidth="1"/>
+    <col min="7" max="9" width="8.72727272727273" style="2"/>
+    <col min="10" max="10" width="16.9090909090909" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="8.72727272727273" style="2"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:10">
@@ -1851,52 +2039,367 @@
       </c>
     </row>
     <row r="2" ht="101.5" spans="1:10">
+      <c r="A2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" ht="116" spans="1:10">
+      <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="20.9090909090909" style="5" customWidth="1"/>
+    <col min="2" max="2" width="21.9090909090909" style="5" customWidth="1"/>
+    <col min="3" max="3" width="59.7272727272727" style="5" customWidth="1"/>
+    <col min="4" max="16384" width="8.72727272727273" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="4" customFormat="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="5">
+        <v>50</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="5">
+        <v>21479</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="B5" s="5">
+        <v>34766</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="6">
+        <v>0.95</v>
+      </c>
+      <c r="B6" s="5">
+        <v>35760</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="6">
+        <v>0.99</v>
+      </c>
+      <c r="B7" s="5">
+        <v>37270</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" s="5">
+        <v>0</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="5">
+        <v>1.2</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="6" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="16.2727272727273" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19.2727272727273" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.6363636363636" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28" style="2" customWidth="1"/>
+    <col min="5" max="5" width="17.9090909090909" style="2" customWidth="1"/>
+    <col min="6" max="6" width="16.3636363636364" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.7272727272727" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.72727272727273" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" ht="58" spans="1:7">
       <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" ht="58" spans="1:7">
+      <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" ht="101.5" spans="1:7">
+      <c r="A4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" ht="87" spans="1:7">
+      <c r="A5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" ht="58" spans="1:7">
+      <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" ht="116" spans="1:9">
-      <c r="A3" t="s">
+      <c r="B6" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" ht="58" spans="1:7">
+      <c r="A7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>36</v>
+      <c r="B7" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>